<commit_message>
se realizan las consultas SQL
</commit_message>
<xml_diff>
--- a/CONSULTAS.xlsx
+++ b/CONSULTAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctobon\Documents\Documentación\1_Programación\Especialización\2do_Semestre\2_Software_Hardware_Big_Data\Trabajo_BD_noSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9247EFA4-5B9E-47B3-8579-0D98E5AA35BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68999EAF-0CB9-474F-9925-F677B3673134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="20490" windowHeight="11385" firstSheet="5" activeTab="6" xr2:uid="{A6C0359A-2E5B-4078-9877-FFB92BF9C795}"/>
+    <workbookView xWindow="1080" yWindow="2250" windowWidth="19320" windowHeight="10350" firstSheet="5" activeTab="5" xr2:uid="{A6C0359A-2E5B-4078-9877-FFB92BF9C795}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENTE" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="134">
   <si>
     <t>nombre_cliente</t>
   </si>
@@ -391,6 +391,57 @@
   </si>
   <si>
     <t>INSERT INTO productos_por_factura(id_producto, id_factura, cantidad, precio) VALUES (3,4,2,7000);</t>
+  </si>
+  <si>
+    <t>fecha_caducidad</t>
+  </si>
+  <si>
+    <t>cantidades_disponibles</t>
+  </si>
+  <si>
+    <t>especialidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2021-03-07'</t>
+  </si>
+  <si>
+    <t>nombre_prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2020-01-01'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2021-04-09'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2020-12-11'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'libra'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'grano'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'bebida'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'condimento'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'carne'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'pasta larga'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'vino'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'pimienta'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'lomo de cerdo'</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1431,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G6" t="str">
-        <f t="shared" ref="G3:G6" si="1">+"INSERT INTO cliente("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;", "&amp;$D$1&amp;", "&amp;$E$1&amp;", "&amp;$F$1&amp;") VALUES ("&amp;A6&amp;","&amp;B6&amp;","&amp;C6&amp;","&amp;D6&amp;","&amp;E6&amp;","&amp;F6&amp;")"</f>
+        <f t="shared" ref="G6" si="1">+"INSERT INTO cliente("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;", "&amp;$D$1&amp;", "&amp;$E$1&amp;", "&amp;$F$1&amp;") VALUES ("&amp;A6&amp;","&amp;B6&amp;","&amp;C6&amp;","&amp;D6&amp;","&amp;E6&amp;","&amp;F6&amp;")"</f>
         <v>INSERT INTO cliente(nombre_producto, precio, especiliadad, medida, unidad_medida, impuesto) VALUES (,,,,,)</v>
       </c>
     </row>
@@ -1411,71 +1462,149 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AF562C-6FCC-41B9-894E-BEF136ED3B99}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="H2" sqref="H2:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="8" width="7.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" t="str">
+        <f>+"INSERT INTO cliente("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;", "&amp;$D$1&amp;", "&amp;$E$1&amp;", "&amp;$F$1&amp;", "&amp;$G$1&amp;") VALUES ("&amp;A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;");"</f>
+        <v>INSERT INTO cliente(fecha_caducidad, cantidades_disponibles, medida, unidad_medida, especialidad, id_sede, nombre_prod) VALUES ( '2020-01-01',20,1, 'libra', 'grano',1, 'pasta larga');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H6" si="0">+"INSERT INTO cliente("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;", "&amp;$D$1&amp;", "&amp;$E$1&amp;", "&amp;$F$1&amp;", "&amp;$G$1&amp;") VALUES ("&amp;A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;");"</f>
+        <v>INSERT INTO cliente(fecha_caducidad, cantidades_disponibles, medida, unidad_medida, especialidad, id_sede, nombre_prod) VALUES ( '2021-03-07',30,500, 'ml', 'bebida',1, 'vino');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO cliente(fecha_caducidad, cantidades_disponibles, medida, unidad_medida, especialidad, id_sede, nombre_prod) VALUES ( '2021-04-09',10,100, 'grs', 'condimento',2, 'pimienta');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I2" t="str">
-        <f>+"INSERT INTO cliente("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;", "&amp;$D$1&amp;", "&amp;$E$1&amp;", "&amp;$F$1&amp;", "&amp;$G$1&amp;","&amp;$H$1&amp;") VALUES ("&amp;A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;")"</f>
-        <v>INSERT INTO cliente(nombre_cliente, apellido_cliente, telefono, direccion, correo, estado_civil, fecha_nacimiento,ciudad) VALUES (,,,,,,,)</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I3" t="str">
-        <f>+"INSERT INTO cliente("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;", "&amp;$D$1&amp;", "&amp;$E$1&amp;", "&amp;$F$1&amp;", "&amp;$G$1&amp;","&amp;$H$1&amp;") VALUES ("&amp;A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;")"</f>
-        <v>INSERT INTO cliente(nombre_cliente, apellido_cliente, telefono, direccion, correo, estado_civil, fecha_nacimiento,ciudad) VALUES (,,,,,,,)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I4" t="str">
-        <f t="shared" ref="I4:I6" si="0">+"INSERT INTO cliente("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;", "&amp;$D$1&amp;", "&amp;$E$1&amp;", "&amp;$F$1&amp;", "&amp;$G$1&amp;","&amp;$H$1&amp;") VALUES ("&amp;A4&amp;","&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;E4&amp;","&amp;F4&amp;","&amp;G4&amp;","&amp;H4&amp;")"</f>
-        <v>INSERT INTO cliente(nombre_cliente, apellido_cliente, telefono, direccion, correo, estado_civil, fecha_nacimiento,ciudad) VALUES (,,,,,,,)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I5" t="str">
+      <c r="G5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO cliente(nombre_cliente, apellido_cliente, telefono, direccion, correo, estado_civil, fecha_nacimiento,ciudad) VALUES (,,,,,,,)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I6" t="str">
+        <v>INSERT INTO cliente(fecha_caducidad, cantidades_disponibles, medida, unidad_medida, especialidad, id_sede, nombre_prod) VALUES ( '2020-12-11',5,1, 'libra', 'carne',3, 'lomo de cerdo');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO cliente(nombre_cliente, apellido_cliente, telefono, direccion, correo, estado_civil, fecha_nacimiento,ciudad) VALUES (,,,,,,,)</v>
+        <v>INSERT INTO cliente(fecha_caducidad, cantidades_disponibles, medida, unidad_medida, especialidad, id_sede, nombre_prod) VALUES (,,,,,,);</v>
       </c>
     </row>
   </sheetData>
@@ -1490,8 +1619,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,8 +1787,8 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>